<commit_message>
update with some filters
</commit_message>
<xml_diff>
--- a/work/compagnb/gap/newHDRQuant.xlsx
+++ b/work/compagnb/gap/newHDRQuant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1260" windowWidth="25760" windowHeight="12160" tabRatio="500"/>
+    <workbookView xWindow="9340" yWindow="1660" windowWidth="19860" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,1047 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="1042">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -380,9 +1418,1047 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="1042">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="437" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="439" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="501" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="503" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="799" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="801" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="803" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="805" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="807" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="809" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="811" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="813" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="815" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="817" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="819" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="821" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="823" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="825" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="827" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="829" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="831" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="835" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="837" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="839" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="841" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="843" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="845" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="847" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="849" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="851" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="853" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="855" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="857" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="859" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="861" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="863" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="865" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="885" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="887" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="889" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="891" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="917" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="919" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="921" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="923" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="925" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="927" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="929" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="931" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="933" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="935" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="937" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="939" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="941" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="943" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="945" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="947" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="949" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="951" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="953" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="955" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="957" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="959" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="961" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="963" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="965" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="967" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="969" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="971" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="973" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="975" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="977" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="979" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="981" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="983" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="985" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="987" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="989" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="991" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="993" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="995" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="997" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="999" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1001" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1003" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1005" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1007" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1009" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1011" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1013" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1015" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1017" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1019" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1021" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1023" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1025" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1027" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1029" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1031" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1033" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1035" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1037" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1039" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1041" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="432" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="434" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="436" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="438" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="500" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="502" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="798" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="800" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="802" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="804" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="806" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="808" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="810" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="812" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="814" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="816" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="818" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="820" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="822" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="824" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="826" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="828" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="830" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="834" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="836" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="838" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="840" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="842" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="844" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="846" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="848" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="850" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="852" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="854" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="856" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="858" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="860" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="862" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="864" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="884" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="886" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="888" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="890" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="916" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="918" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="920" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="922" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="924" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="926" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="928" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="930" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="932" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="934" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="936" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="938" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="940" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="942" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="944" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="946" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="948" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="950" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="952" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="954" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="956" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="958" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="960" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="962" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="964" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="966" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="968" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="970" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="972" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="974" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="976" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="978" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="980" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="982" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="984" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="986" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="988" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="990" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="992" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="994" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="996" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="998" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1000" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1002" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1004" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1006" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1008" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1010" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1012" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1014" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1016" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1018" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1020" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1022" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1024" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1026" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1028" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1030" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1032" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1034" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1036" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1038" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1040" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
@@ -715,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2030,7 +4106,7 @@
         <v>3214.6219620589022</v>
       </c>
       <c r="M32" s="8">
-        <v>10691.702139954697</v>
+        <v>10691.702139954699</v>
       </c>
       <c r="N32" s="7"/>
     </row>
@@ -2316,7 +4392,7 @@
         <v>12.7</v>
       </c>
       <c r="L39" s="8">
-        <v>1454.9714389853627</v>
+        <v>1454.97143898536</v>
       </c>
       <c r="M39" s="8">
         <v>1998.5015278960225</v>

</xml_diff>